<commit_message>
added script for failing a tese case
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>umang8880@up.com</t>
   </si>
   <si>
-    <t>Lightning Experience</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>8460343563</t>
+  </si>
+  <si>
+    <t>Lightning</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -508,13 +508,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -524,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -536,96 +536,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>